<commit_message>
Add R probability book
</commit_message>
<xml_diff>
--- a/materials/Week3Questions.xlsx
+++ b/materials/Week3Questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cimacint\Documents\GitHub\statistics\materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cimac\OneDrive\Documents\GitHub\statistics\materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EDEACA-3001-4D5C-ABDF-4ED49F957B7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{52EDEACA-3001-4D5C-ABDF-4ED49F957B7F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{70A00BD7-EE43-4EB9-8182-69D5D098DB7F}"/>
   <bookViews>
-    <workbookView xWindow="650" yWindow="370" windowWidth="20980" windowHeight="10750" xr2:uid="{F51AF9FE-1576-4C0C-B963-4870BE35EA56}"/>
+    <workbookView xWindow="1608" yWindow="264" windowWidth="19572" windowHeight="11724" xr2:uid="{F51AF9FE-1576-4C0C-B963-4870BE35EA56}"/>
   </bookViews>
   <sheets>
     <sheet name="Quiz" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="484">
   <si>
     <t>https://www.youtube.com/watch?v=1PsPfMaLWSk</t>
   </si>
@@ -1371,6 +1371,117 @@
   </si>
   <si>
     <t>dependent</t>
+  </si>
+  <si>
+    <t>zscore</t>
+  </si>
+  <si>
+    <t>What does centering a variable mean?</t>
+  </si>
+  <si>
+    <t>How do you center a variable?</t>
+  </si>
+  <si>
+    <t>subtract the mean from each score</t>
+  </si>
+  <si>
+    <t>subtract the standard deviation from each score</t>
+  </si>
+  <si>
+    <t>fix the formatting for the column in your spreadsheet</t>
+  </si>
+  <si>
+    <t>Why would you want to center a variable?</t>
+  </si>
+  <si>
+    <t>it makes it easier to interpret</t>
+  </si>
+  <si>
+    <t>moving the mean of the variable scores to zero by subtracting the mean from each score</t>
+  </si>
+  <si>
+    <t>making the variable easier to interpret by moving the mean to zero</t>
+  </si>
+  <si>
+    <t>moving your computer so it's in the center of your desk</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>all the other statisticians are doing it</t>
+  </si>
+  <si>
+    <t>making scores bigger than the mean greater than zero</t>
+  </si>
+  <si>
+    <t>making scores less than the mean less than zero</t>
+  </si>
+  <si>
+    <t>1,2,4,5</t>
+  </si>
+  <si>
+    <t>it's easier to interpret because scores greater than zero are greater than the mean after they're centered.</t>
+  </si>
+  <si>
+    <t>it's easier to interpret because scores less than zero are smaller than the mean after they're centered.</t>
+  </si>
+  <si>
+    <t>1,3,4</t>
+  </si>
+  <si>
+    <t>What is the mean for variables that have been converted to a Z score?</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>the same as the original variable</t>
+  </si>
+  <si>
+    <t>What units are z scores in?</t>
+  </si>
+  <si>
+    <t>standard deviations</t>
+  </si>
+  <si>
+    <t>the original unit of measurement</t>
+  </si>
+  <si>
+    <t>Why are z scores useful?</t>
+  </si>
+  <si>
+    <t>They allow you to compare variables that were measured on different scales.</t>
+  </si>
+  <si>
+    <t>They make interpreting scores easier.</t>
+  </si>
+  <si>
+    <t>They're more accurate than raw scores.</t>
+  </si>
+  <si>
+    <t>What is the standard deviation for z scores?</t>
+  </si>
+  <si>
+    <t>there are no units for z scores.</t>
+  </si>
+  <si>
+    <t>What do percentiles tell us?</t>
+  </si>
+  <si>
+    <t>The percentage of scores that are lower than or equal to the z score of interest.</t>
+  </si>
+  <si>
+    <t>The percent correct on a test.</t>
+  </si>
+  <si>
+    <t>How to calculate percentages.</t>
+  </si>
+  <si>
+    <t>percentile</t>
   </si>
 </sst>
 </file>
@@ -1727,20 +1838,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F54A43F-FA7D-40F7-85DB-59E611BE8551}">
   <dimension ref="A1:AH225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29:C33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" customWidth="1"/>
-    <col min="4" max="4" width="23.08984375" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" customWidth="1"/>
-    <col min="17" max="17" width="20.36328125" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="17" max="17" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>347</v>
       </c>
@@ -1844,7 +1955,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
         <v>390</v>
       </c>
@@ -1870,7 +1981,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>390</v>
       </c>
@@ -1896,7 +2007,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>390</v>
       </c>
@@ -1922,7 +2033,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>390</v>
       </c>
@@ -1948,7 +2059,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>390</v>
       </c>
@@ -1974,7 +2085,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>390</v>
       </c>
@@ -2000,7 +2111,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>390</v>
       </c>
@@ -2023,7 +2134,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>390</v>
       </c>
@@ -2046,7 +2157,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>410</v>
       </c>
@@ -2072,7 +2183,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>410</v>
       </c>
@@ -2098,7 +2209,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>410</v>
       </c>
@@ -2124,7 +2235,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>410</v>
       </c>
@@ -2150,7 +2261,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>410</v>
       </c>
@@ -2176,7 +2287,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>410</v>
       </c>
@@ -2202,7 +2313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>410</v>
       </c>
@@ -2228,7 +2339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>410</v>
       </c>
@@ -2254,7 +2365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>410</v>
       </c>
@@ -2280,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>410</v>
       </c>
@@ -2306,7 +2417,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>410</v>
       </c>
@@ -2337,7 +2448,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>410</v>
       </c>
@@ -2368,7 +2479,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>410</v>
       </c>
@@ -2399,7 +2510,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>410</v>
       </c>
@@ -2430,7 +2541,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>410</v>
       </c>
@@ -2461,7 +2572,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>410</v>
       </c>
@@ -2490,7 +2601,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>410</v>
       </c>
@@ -2521,7 +2632,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>410</v>
       </c>
@@ -2550,7 +2661,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>438</v>
       </c>
@@ -2570,7 +2681,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>438</v>
       </c>
@@ -2590,7 +2701,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
         <v>438</v>
       </c>
@@ -2610,7 +2721,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>438</v>
       </c>
@@ -2630,7 +2741,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>438</v>
       </c>
@@ -2650,7 +2761,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>438</v>
       </c>
@@ -2670,12 +2781,181 @@
         <v>158</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>447</v>
+      </c>
+      <c r="D34" t="s">
+        <v>448</v>
+      </c>
+      <c r="E34" t="s">
+        <v>462</v>
+      </c>
+      <c r="F34" t="s">
+        <v>455</v>
+      </c>
+      <c r="G34" t="s">
+        <v>456</v>
+      </c>
+      <c r="H34" t="s">
+        <v>457</v>
+      </c>
+      <c r="I34" t="s">
+        <v>460</v>
+      </c>
+      <c r="J34" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>447</v>
+      </c>
+      <c r="D35" t="s">
+        <v>449</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>450</v>
+      </c>
+      <c r="G35" t="s">
+        <v>451</v>
+      </c>
+      <c r="H35" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>447</v>
+      </c>
+      <c r="D36" t="s">
+        <v>453</v>
+      </c>
+      <c r="E36" t="s">
+        <v>465</v>
+      </c>
+      <c r="F36" t="s">
+        <v>454</v>
+      </c>
+      <c r="G36" t="s">
+        <v>459</v>
+      </c>
+      <c r="H36" t="s">
+        <v>463</v>
+      </c>
+      <c r="I36" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>447</v>
+      </c>
+      <c r="D37" t="s">
+        <v>466</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>467</v>
+      </c>
+      <c r="G37" t="s">
+        <v>468</v>
+      </c>
+      <c r="H37" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>447</v>
+      </c>
+      <c r="D38" t="s">
+        <v>470</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>471</v>
+      </c>
+      <c r="G38" t="s">
+        <v>472</v>
+      </c>
+      <c r="H38" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>447</v>
+      </c>
+      <c r="D39" t="s">
+        <v>473</v>
+      </c>
+      <c r="E39" t="s">
+        <v>458</v>
+      </c>
+      <c r="F39" t="s">
+        <v>474</v>
+      </c>
+      <c r="G39" t="s">
+        <v>475</v>
+      </c>
+      <c r="H39" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>447</v>
+      </c>
+      <c r="D40" t="s">
+        <v>477</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>467</v>
+      </c>
+      <c r="G40" t="s">
+        <v>468</v>
+      </c>
+      <c r="H40" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>483</v>
+      </c>
+      <c r="D41" t="s">
+        <v>479</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>480</v>
+      </c>
+      <c r="G41" t="s">
+        <v>481</v>
+      </c>
+      <c r="H41" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>381</v>
       </c>
@@ -2695,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>381</v>
       </c>
@@ -2715,7 +2995,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>381</v>
       </c>
@@ -2735,7 +3015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>381</v>
       </c>
@@ -2755,7 +3035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>381</v>
       </c>
@@ -2775,7 +3055,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>381</v>
       </c>
@@ -2795,7 +3075,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>381</v>
       </c>
@@ -2815,7 +3095,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>382</v>
       </c>
@@ -2847,7 +3127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>381</v>
       </c>
@@ -2867,7 +3147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>381</v>
       </c>
@@ -2887,7 +3167,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>381</v>
       </c>
@@ -2907,7 +3187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>381</v>
       </c>
@@ -2927,7 +3207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>381</v>
       </c>
@@ -2947,7 +3227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>381</v>
       </c>
@@ -2967,7 +3247,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>381</v>
       </c>
@@ -2987,7 +3267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>381</v>
       </c>
@@ -3007,7 +3287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>381</v>
       </c>
@@ -3027,7 +3307,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>381</v>
       </c>
@@ -3047,7 +3327,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>381</v>
       </c>
@@ -3067,7 +3347,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>381</v>
       </c>
@@ -3087,7 +3367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>382</v>
       </c>
@@ -3122,7 +3402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>381</v>
       </c>
@@ -3142,7 +3422,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>381</v>
       </c>
@@ -3162,7 +3442,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>382</v>
       </c>
@@ -3197,7 +3477,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>381</v>
       </c>
@@ -3217,7 +3497,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>381</v>
       </c>
@@ -3237,7 +3517,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>381</v>
       </c>
@@ -3257,7 +3537,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>381</v>
       </c>
@@ -3277,7 +3557,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>381</v>
       </c>
@@ -3297,7 +3577,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>381</v>
       </c>
@@ -3317,7 +3597,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>381</v>
       </c>
@@ -3337,7 +3617,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>381</v>
       </c>
@@ -3357,7 +3637,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>381</v>
       </c>
@@ -3377,7 +3657,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>383</v>
       </c>
@@ -3427,7 +3707,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>383</v>
       </c>
@@ -3477,7 +3757,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>383</v>
       </c>
@@ -3509,7 +3789,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>383</v>
       </c>
@@ -3547,7 +3827,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>381</v>
       </c>
@@ -3567,7 +3847,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>381</v>
       </c>
@@ -3587,7 +3867,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>381</v>
       </c>
@@ -3607,7 +3887,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>381</v>
       </c>
@@ -3627,7 +3907,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>381</v>
       </c>
@@ -3647,7 +3927,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>381</v>
       </c>
@@ -3667,7 +3947,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>382</v>
       </c>
@@ -3696,7 +3976,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>382</v>
       </c>
@@ -3725,7 +4005,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>382</v>
       </c>
@@ -3754,7 +4034,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>382</v>
       </c>
@@ -3783,7 +4063,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>382</v>
       </c>
@@ -3812,7 +4092,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>382</v>
       </c>
@@ -3841,7 +4121,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>382</v>
       </c>
@@ -3870,7 +4150,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>382</v>
       </c>
@@ -3899,7 +4179,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>382</v>
       </c>
@@ -3928,7 +4208,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>382</v>
       </c>
@@ -3957,7 +4237,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>382</v>
       </c>
@@ -3986,7 +4266,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>383</v>
       </c>
@@ -4036,7 +4316,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>383</v>
       </c>
@@ -4083,7 +4363,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>383</v>
       </c>
@@ -4121,7 +4401,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>383</v>
       </c>
@@ -4159,7 +4439,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>383</v>
       </c>
@@ -4209,7 +4489,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>383</v>
       </c>
@@ -4259,7 +4539,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>383</v>
       </c>
@@ -4309,7 +4589,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>383</v>
       </c>
@@ -4359,7 +4639,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>381</v>
       </c>
@@ -4379,7 +4659,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>381</v>
       </c>
@@ -4399,7 +4679,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>382</v>
       </c>
@@ -4434,7 +4714,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>382</v>
       </c>
@@ -4469,7 +4749,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>382</v>
       </c>
@@ -4504,7 +4784,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>382</v>
       </c>
@@ -4539,7 +4819,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>381</v>
       </c>
@@ -4559,7 +4839,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>381</v>
       </c>
@@ -4579,7 +4859,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>381</v>
       </c>
@@ -4599,7 +4879,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>381</v>
       </c>
@@ -4619,7 +4899,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>381</v>
       </c>
@@ -4639,7 +4919,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>381</v>
       </c>
@@ -4659,7 +4939,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>381</v>
       </c>
@@ -4679,7 +4959,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>381</v>
       </c>
@@ -4699,7 +4979,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>381</v>
       </c>
@@ -4719,7 +4999,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>381</v>
       </c>
@@ -4739,7 +5019,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>381</v>
       </c>
@@ -4759,7 +5039,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>381</v>
       </c>
@@ -4779,7 +5059,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>381</v>
       </c>
@@ -4799,7 +5079,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>381</v>
       </c>
@@ -4819,7 +5099,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>381</v>
       </c>
@@ -4839,7 +5119,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>381</v>
       </c>
@@ -4859,7 +5139,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>381</v>
       </c>
@@ -4879,7 +5159,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>381</v>
       </c>
@@ -4899,7 +5179,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>381</v>
       </c>
@@ -4919,7 +5199,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>381</v>
       </c>
@@ -4939,7 +5219,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>381</v>
       </c>
@@ -4959,7 +5239,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>381</v>
       </c>
@@ -4979,7 +5259,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>381</v>
       </c>
@@ -4999,7 +5279,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>381</v>
       </c>
@@ -5019,7 +5299,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>381</v>
       </c>
@@ -5039,7 +5319,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>381</v>
       </c>
@@ -5059,7 +5339,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>382</v>
       </c>
@@ -5094,7 +5374,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>382</v>
       </c>
@@ -5129,7 +5409,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>382</v>
       </c>
@@ -5164,7 +5444,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>382</v>
       </c>
@@ -5199,7 +5479,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>382</v>
       </c>
@@ -5234,7 +5514,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>382</v>
       </c>
@@ -5269,7 +5549,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>382</v>
       </c>
@@ -5304,7 +5584,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>382</v>
       </c>
@@ -5339,7 +5619,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>382</v>
       </c>
@@ -5374,7 +5654,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>382</v>
       </c>
@@ -5409,7 +5689,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>382</v>
       </c>
@@ -5444,7 +5724,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>382</v>
       </c>
@@ -5479,7 +5759,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>382</v>
       </c>
@@ -5514,7 +5794,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>382</v>
       </c>
@@ -5549,7 +5829,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>382</v>
       </c>
@@ -5584,7 +5864,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>382</v>
       </c>
@@ -5619,7 +5899,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>382</v>
       </c>
@@ -5654,7 +5934,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>382</v>
       </c>
@@ -5689,7 +5969,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>382</v>
       </c>
@@ -5724,7 +6004,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>382</v>
       </c>
@@ -5759,7 +6039,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>382</v>
       </c>
@@ -5794,7 +6074,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>382</v>
       </c>
@@ -5829,7 +6109,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>382</v>
       </c>
@@ -5864,7 +6144,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>382</v>
       </c>
@@ -5899,7 +6179,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>382</v>
       </c>
@@ -5934,7 +6214,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>382</v>
       </c>
@@ -5969,7 +6249,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>382</v>
       </c>
@@ -6004,7 +6284,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>382</v>
       </c>
@@ -6039,7 +6319,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>382</v>
       </c>
@@ -6074,7 +6354,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>382</v>
       </c>
@@ -6109,7 +6389,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>382</v>
       </c>
@@ -6144,7 +6424,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>382</v>
       </c>

</xml_diff>